<commit_message>
Add extra "testng.xml" for suite level test execution
</commit_message>
<xml_diff>
--- a/Orange/src/test/resources/data/loginData.xlsx
+++ b/Orange/src/test/resources/data/loginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\Orange\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\OrangeHRM\Orange\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339F3015-4DDD-49D7-A226-8FEC971A11E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA00507C-7B29-466D-9D75-7984D9B6294A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Admin</t>
   </si>
   <si>
     <t>admin123</t>
-  </si>
-  <si>
-    <t>nimda321</t>
-  </si>
-  <si>
-    <t>nimdA</t>
   </si>
   <si>
     <t>username</t>
@@ -375,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -388,10 +382,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -402,30 +396,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>